<commit_message>
updated lookup table vc
</commit_message>
<xml_diff>
--- a/setups/vestibular chair/vPrime/lookup/lookup_VC.xlsx
+++ b/setups/vestibular chair/vPrime/lookup/lookup_VC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjheckman/Documents/Code/Gitlab/pbtoolbox/setups/vestibular chair/vPrime/lookup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BBC2ACFC-DCB2-814C-8684-9E67D33CAB34}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712A2F98-B4BD-F645-A631-77421348ED2A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="4320" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{5850A143-55FE-1E4C-9912-3283C1074301}"/>
+    <workbookView xWindow="5560" yWindow="2640" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{5850A143-55FE-1E4C-9912-3283C1074301}"/>
   </bookViews>
   <sheets>
     <sheet name="Visual Map" sheetId="1" r:id="rId1"/>
@@ -460,10 +460,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18420191-E37D-8D45-99AD-5697EE511741}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A17"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -604,6 +604,14 @@
         <v>17</v>
       </c>
     </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18" s="2">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>